<commit_message>
update BOM - added 2.2uf Cap and BAT46 diode
</commit_message>
<xml_diff>
--- a/docs/Mirto_BOM.xlsx
+++ b/docs/Mirto_BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\Documents\github\Mirto2023\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06CBCA29-1DF9-4FE5-8289-46D82B65AD9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{380B36FD-5778-4F55-B1B9-4CB75BF0AE46}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26445" yWindow="1860" windowWidth="25493" windowHeight="13208" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1970" yWindow="920" windowWidth="28800" windowHeight="15460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mirto2023" sheetId="7" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="75">
   <si>
     <t>Quantity (per robot)</t>
   </si>
@@ -253,6 +253,12 @@
   </si>
   <si>
     <t xml:space="preserve">	2886085</t>
+  </si>
+  <si>
+    <t>BAT46</t>
+  </si>
+  <si>
+    <t>2.2uF cap</t>
   </si>
 </sst>
 </file>
@@ -373,7 +379,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -412,6 +418,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,9 +437,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -470,9 +477,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -505,26 +512,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -557,26 +547,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -750,23 +723,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4A27733-5134-4884-92DD-DF33C91E4474}">
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="C6:D6"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.3984375" customWidth="1"/>
-    <col min="2" max="2" width="15.59765625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.3984375" customWidth="1"/>
-    <col min="4" max="4" width="14.265625" customWidth="1"/>
-    <col min="5" max="5" width="14.59765625" customWidth="1"/>
-    <col min="6" max="6" width="44.3984375" customWidth="1"/>
+    <col min="1" max="1" width="30.36328125" customWidth="1"/>
+    <col min="2" max="2" width="15.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.36328125" customWidth="1"/>
+    <col min="4" max="4" width="14.26953125" customWidth="1"/>
+    <col min="5" max="5" width="14.6328125" customWidth="1"/>
+    <col min="6" max="6" width="44.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="10" t="s">
         <v>59</v>
       </c>
@@ -778,7 +751,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -796,7 +769,7 @@
       </c>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>30</v>
       </c>
@@ -806,7 +779,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -817,7 +790,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="3">
-        <f t="shared" ref="D5:D19" si="0">$D$1*C5</f>
+        <f t="shared" ref="D5:D21" si="0">$D$1*C5</f>
         <v>30</v>
       </c>
       <c r="E5" s="14"/>
@@ -825,7 +798,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -839,7 +812,7 @@
       <c r="E6" s="14"/>
       <c r="F6" s="3"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>5</v>
       </c>
@@ -859,7 +832,7 @@
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -879,29 +852,32 @@
       <c r="H8" s="3"/>
       <c r="I8" s="3"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="4">
+        <v>1827838</v>
+      </c>
+      <c r="C9" s="3">
+        <v>1</v>
+      </c>
+      <c r="D9" s="3">
+        <f>$D$1*C9</f>
+        <v>15</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16"/>
+      <c r="I9" s="16"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B10" s="4">
         <v>9356100</v>
-      </c>
-      <c r="C9" s="3">
-        <v>2</v>
-      </c>
-      <c r="D9" s="3">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="E9" s="14"/>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A10" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="B10" s="6">
-        <v>1829197</v>
       </c>
       <c r="C10" s="3">
         <v>2</v>
@@ -910,33 +886,32 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="E10" s="3"/>
+      <c r="E10" s="14"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="7">
-        <v>1201431</v>
+        <v>61</v>
+      </c>
+      <c r="B11" s="6">
+        <v>1829197</v>
       </c>
       <c r="C11" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" s="3">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
-      <c r="H11" s="2"/>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B12" s="6">
-        <v>9843680</v>
+        <v>9</v>
+      </c>
+      <c r="B12" s="7">
+        <v>1201431</v>
       </c>
       <c r="C12" s="3">
         <v>1</v>
@@ -949,12 +924,12 @@
       <c r="F12" s="3"/>
       <c r="H12" s="2"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13" s="4">
-        <v>1581112</v>
+        <v>17</v>
+      </c>
+      <c r="B13" s="6">
+        <v>9843680</v>
       </c>
       <c r="C13" s="3">
         <v>1</v>
@@ -965,15 +940,16 @@
       </c>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H13" s="2"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B14" s="4">
-        <v>1581114</v>
-      </c>
-      <c r="C14" s="8">
+        <v>73</v>
+      </c>
+      <c r="B14" s="6">
+        <v>9801456</v>
+      </c>
+      <c r="C14" s="3">
         <v>1</v>
       </c>
       <c r="D14" s="3">
@@ -982,15 +958,16 @@
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="H14" s="2"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="6">
-        <v>1593463</v>
-      </c>
-      <c r="C15" s="8">
+        <v>10</v>
+      </c>
+      <c r="B15" s="4">
+        <v>1581112</v>
+      </c>
+      <c r="C15" s="3">
         <v>1</v>
       </c>
       <c r="D15" s="3">
@@ -1000,12 +977,12 @@
       <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" s="6">
-        <v>1593462</v>
+        <v>11</v>
+      </c>
+      <c r="B16" s="4">
+        <v>1581114</v>
       </c>
       <c r="C16" s="8">
         <v>1</v>
@@ -1017,29 +994,29 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
-        <v>65</v>
+        <v>21</v>
       </c>
       <c r="B17" s="6">
-        <v>1593469</v>
+        <v>1593463</v>
       </c>
       <c r="C17" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D17" s="3">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B18" s="6" t="s">
-        <v>70</v>
+        <v>36</v>
+      </c>
+      <c r="B18" s="6">
+        <v>1593462</v>
       </c>
       <c r="C18" s="8">
         <v>1</v>
@@ -1051,89 +1028,84 @@
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B19" s="6" t="s">
-        <v>72</v>
+        <v>65</v>
+      </c>
+      <c r="B19" s="6">
+        <v>1593469</v>
       </c>
       <c r="C19" s="8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D19" s="3">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="3"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B20" s="4">
-        <v>9491848</v>
+        <v>69</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>70</v>
       </c>
       <c r="C20" s="8">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D20" s="3">
-        <f t="shared" ref="D20:D25" si="2">$D$1*C20</f>
-        <v>30</v>
+        <f t="shared" si="0"/>
+        <v>15</v>
       </c>
       <c r="E20" s="3"/>
-      <c r="F20" s="3" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="F20" s="3"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B21" s="4">
-        <v>224959</v>
+        <v>71</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>72</v>
       </c>
       <c r="C21" s="8">
         <v>1</v>
       </c>
       <c r="D21" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="3">
-        <v>1</v>
+        <v>12</v>
+      </c>
+      <c r="B22" s="4">
+        <v>9491848</v>
+      </c>
+      <c r="C22" s="8">
+        <v>2</v>
       </c>
       <c r="D22" s="3">
-        <f t="shared" si="2"/>
-        <v>15</v>
+        <f t="shared" ref="D22:D27" si="2">$D$1*C22</f>
+        <v>30</v>
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B23" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="C23" s="3">
+        <v>37</v>
+      </c>
+      <c r="B23" s="4">
+        <v>224959</v>
+      </c>
+      <c r="C23" s="8">
         <v>1</v>
       </c>
       <c r="D23" s="3">
@@ -1141,16 +1113,14 @@
         <v>15</v>
       </c>
       <c r="E23" s="3"/>
-      <c r="F23" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B24" s="15" t="s">
-        <v>67</v>
+        <v>18</v>
+      </c>
+      <c r="B24" s="9" t="s">
+        <v>19</v>
       </c>
       <c r="C24" s="3">
         <v>1</v>
@@ -1161,14 +1131,19 @@
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="3" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+        <v>38</v>
+      </c>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="3"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B25" s="9"/>
+        <v>62</v>
+      </c>
+      <c r="B25" s="15" t="s">
+        <v>63</v>
+      </c>
       <c r="C25" s="3">
         <v>1</v>
       </c>
@@ -1178,87 +1153,87 @@
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B26" s="4"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="3"/>
+        <v>66</v>
+      </c>
+      <c r="B26" s="15" t="s">
+        <v>67</v>
+      </c>
+      <c r="C26" s="3">
+        <v>1</v>
+      </c>
+      <c r="D26" s="3">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
       <c r="E26" s="3"/>
       <c r="F26" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A27" s="3"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="3"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B27" s="9"/>
+      <c r="C27" s="3">
+        <v>1</v>
+      </c>
+      <c r="D27" s="3">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
       <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A28" s="5" t="s">
-        <v>43</v>
+      <c r="F27" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="B28" s="4"/>
       <c r="C28" s="8"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A29" s="3" t="s">
+      <c r="F28" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" s="3"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B30" s="4"/>
+      <c r="C30" s="8"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A31" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="4">
+      <c r="B31" s="4">
         <v>1420391</v>
       </c>
-      <c r="C29" s="8">
-        <v>4</v>
-      </c>
-      <c r="D29" s="3">
-        <f t="shared" ref="D29:D37" si="3">$D$1*C29</f>
-        <v>60</v>
-      </c>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A30" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B30" s="4">
-        <v>1419987</v>
-      </c>
-      <c r="C30" s="8">
-        <v>12</v>
-      </c>
-      <c r="D30" s="3">
-        <f t="shared" si="3"/>
-        <v>180</v>
-      </c>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A31" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B31" s="4"/>
       <c r="C31" s="8">
         <v>4</v>
       </c>
       <c r="D31" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" ref="D31:D39" si="3">$D$1*C31</f>
         <v>60</v>
       </c>
       <c r="E31" s="3"/>
@@ -1266,176 +1241,194 @@
         <v>26</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B32" s="4">
-        <v>1419447</v>
+        <v>1419987</v>
       </c>
       <c r="C32" s="8">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="D32" s="3">
         <f t="shared" si="3"/>
-        <v>240</v>
+        <v>180</v>
       </c>
       <c r="E32" s="3"/>
       <c r="F32" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B33" s="4">
-        <v>1419992</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="B33" s="4"/>
       <c r="C33" s="8">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D33" s="3">
         <f t="shared" si="3"/>
-        <v>90</v>
+        <v>60</v>
       </c>
       <c r="E33" s="3"/>
       <c r="F33" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A34" s="3"/>
-      <c r="B34" s="4"/>
-      <c r="C34" s="8"/>
-      <c r="D34" s="3"/>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A34" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B34" s="4">
+        <v>1419447</v>
+      </c>
+      <c r="C34" s="8">
+        <v>16</v>
+      </c>
+      <c r="D34" s="3">
+        <f t="shared" si="3"/>
+        <v>240</v>
+      </c>
       <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="F34" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B35" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
+      </c>
+      <c r="B35" s="4">
+        <v>1419992</v>
       </c>
       <c r="C35" s="8">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D35" s="3">
         <f t="shared" si="3"/>
-        <v>30</v>
+        <v>90</v>
       </c>
       <c r="E35" s="3"/>
       <c r="F35" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" s="3"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="8"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="C37" s="8">
+        <v>2</v>
+      </c>
+      <c r="D37" s="3">
+        <f t="shared" si="3"/>
+        <v>30</v>
+      </c>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A36" s="3" t="s">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B36" s="4"/>
-      <c r="C36" s="8">
-        <v>1</v>
-      </c>
-      <c r="D36" s="3">
+      <c r="B38" s="4"/>
+      <c r="C38" s="8">
+        <v>1</v>
+      </c>
+      <c r="D38" s="3">
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3" t="s">
+      <c r="E38" s="3"/>
+      <c r="F38" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A37" s="3" t="s">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B37" s="4"/>
-      <c r="C37" s="8">
-        <v>1</v>
-      </c>
-      <c r="D37" s="3">
+      <c r="B39" s="4"/>
+      <c r="C39" s="8">
+        <v>1</v>
+      </c>
+      <c r="D39" s="3">
         <f t="shared" si="3"/>
         <v>15</v>
       </c>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A38" s="3"/>
-      <c r="B38" s="4"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="3"/>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A39" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="B39" s="4"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="3"/>
       <c r="E39" s="3"/>
       <c r="F39" s="3" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A40" s="3" t="s">
-        <v>55</v>
-      </c>
+        <v>52</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" s="3"/>
       <c r="B40" s="4"/>
-      <c r="C40" s="8">
-        <v>2</v>
-      </c>
-      <c r="D40" s="3">
-        <f t="shared" ref="D40:D41" si="4">$D$1*C40</f>
-        <v>30</v>
-      </c>
+      <c r="C40" s="8"/>
+      <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A41" s="3" t="s">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A41" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B41" s="4"/>
+      <c r="C41" s="8"/>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A42" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B42" s="4"/>
+      <c r="C42" s="8">
+        <v>2</v>
+      </c>
+      <c r="D42" s="3">
+        <f t="shared" ref="D42:D43" si="4">$D$1*C42</f>
+        <v>30</v>
+      </c>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A43" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B41" s="4"/>
-      <c r="C41" s="8">
+      <c r="B43" s="4"/>
+      <c r="C43" s="8">
         <v>2</v>
       </c>
-      <c r="D41" s="3">
+      <c r="D43" s="3">
         <f t="shared" si="4"/>
         <v>30</v>
       </c>
-      <c r="E41" s="3"/>
-      <c r="F41" s="3"/>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A42" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B42" s="4"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="3"/>
-      <c r="E42" s="3"/>
-      <c r="F42" s="3"/>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A43" s="3"/>
-      <c r="B43" s="4"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="3"/>
       <c r="E43" s="3"/>
       <c r="F43" s="3"/>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A44" s="5" t="s">
-        <v>58</v>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A44" s="3" t="s">
+        <v>57</v>
       </c>
       <c r="B44" s="4"/>
       <c r="C44" s="8"/>
@@ -1443,45 +1436,63 @@
       <c r="E44" s="3"/>
       <c r="F44" s="3"/>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A45" s="3" t="s">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A45" s="3"/>
+      <c r="B45" s="4"/>
+      <c r="C45" s="8"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A46" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B46" s="4"/>
+      <c r="C46" s="8"/>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A47" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B45" s="9" t="s">
+      <c r="B47" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F45" s="3"/>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A46" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B46" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C46" s="3"/>
-      <c r="D46" s="3"/>
-      <c r="E46" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F46" s="3"/>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A47" s="3"/>
-      <c r="B47" s="4"/>
       <c r="C47" s="3"/>
       <c r="D47" s="3"/>
-      <c r="E47" s="3"/>
+      <c r="E47" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="F47" s="3"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A48" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C48" s="3"/>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F48" s="3"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A49" s="3"/>
+      <c r="B49" s="4"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1493,17 +1504,17 @@
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.3984375" customWidth="1"/>
-    <col min="2" max="2" width="15.59765625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.3984375" customWidth="1"/>
-    <col min="4" max="4" width="14.265625" customWidth="1"/>
-    <col min="5" max="5" width="14.59765625" customWidth="1"/>
-    <col min="6" max="6" width="44.3984375" customWidth="1"/>
+    <col min="1" max="1" width="30.36328125" customWidth="1"/>
+    <col min="2" max="2" width="15.6328125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.36328125" customWidth="1"/>
+    <col min="4" max="4" width="14.26953125" customWidth="1"/>
+    <col min="5" max="5" width="14.6328125" customWidth="1"/>
+    <col min="6" max="6" width="44.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:8" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="10" t="s">
         <v>29</v>
       </c>
@@ -1515,7 +1526,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1533,7 +1544,7 @@
       </c>
       <c r="F3" s="3"/>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="5" t="s">
         <v>30</v>
       </c>
@@ -1543,7 +1554,7 @@
       <c r="E4" s="4"/>
       <c r="F4" s="3"/>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>6</v>
       </c>
@@ -1564,7 +1575,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>33</v>
       </c>
@@ -1585,7 +1596,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>34</v>
       </c>
@@ -1602,7 +1613,7 @@
       <c r="E7" s="14"/>
       <c r="F7" s="3"/>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>35</v>
       </c>
@@ -1619,7 +1630,7 @@
       <c r="E8" s="3"/>
       <c r="F8" s="3"/>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>9</v>
       </c>
@@ -1637,7 +1648,7 @@
       <c r="F9" s="3"/>
       <c r="H9" s="2"/>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>10</v>
       </c>
@@ -1654,7 +1665,7 @@
       <c r="E10" s="3"/>
       <c r="F10" s="3"/>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>11</v>
       </c>
@@ -1671,7 +1682,7 @@
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>28</v>
       </c>
@@ -1688,7 +1699,7 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>21</v>
       </c>
@@ -1705,7 +1716,7 @@
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>36</v>
       </c>
@@ -1722,7 +1733,7 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>12</v>
       </c>
@@ -1741,7 +1752,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>37</v>
       </c>
@@ -1758,7 +1769,7 @@
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>18</v>
       </c>
@@ -1780,7 +1791,7 @@
       <c r="H17" s="3"/>
       <c r="I17" s="3"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>39</v>
       </c>
@@ -1797,7 +1808,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
         <v>41</v>
       </c>
@@ -1809,7 +1820,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="4"/>
       <c r="C20" s="8"/>
@@ -1817,7 +1828,7 @@
       <c r="E20" s="3"/>
       <c r="F20" s="3"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="5" t="s">
         <v>43</v>
       </c>
@@ -1827,7 +1838,7 @@
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="3" t="s">
         <v>15</v>
       </c>
@@ -1846,7 +1857,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>14</v>
       </c>
@@ -1865,7 +1876,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="3" t="s">
         <v>44</v>
       </c>
@@ -1882,7 +1893,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>16</v>
       </c>
@@ -1901,7 +1912,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="3" t="s">
         <v>45</v>
       </c>
@@ -1920,7 +1931,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="3"/>
       <c r="B27" s="4"/>
       <c r="C27" s="8"/>
@@ -1928,7 +1939,7 @@
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>46</v>
       </c>
@@ -1947,7 +1958,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="3" t="s">
         <v>49</v>
       </c>
@@ -1964,7 +1975,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>51</v>
       </c>
@@ -1981,7 +1992,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
       <c r="B31" s="4"/>
       <c r="C31" s="8"/>
@@ -1989,7 +2000,7 @@
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="5" t="s">
         <v>53</v>
       </c>
@@ -2001,7 +2012,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" s="3" t="s">
         <v>55</v>
       </c>
@@ -2016,7 +2027,7 @@
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" s="3" t="s">
         <v>56</v>
       </c>
@@ -2031,7 +2042,7 @@
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35" s="3" t="s">
         <v>57</v>
       </c>
@@ -2041,7 +2052,7 @@
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36" s="3"/>
       <c r="B36" s="4"/>
       <c r="C36" s="8"/>
@@ -2049,7 +2060,7 @@
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37" s="5" t="s">
         <v>58</v>
       </c>
@@ -2059,7 +2070,7 @@
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A38" s="3" t="s">
         <v>25</v>
       </c>
@@ -2073,7 +2084,7 @@
       </c>
       <c r="F38" s="3"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A39" s="3" t="s">
         <v>23</v>
       </c>
@@ -2087,7 +2098,7 @@
       </c>
       <c r="F39" s="3"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A40" s="3"/>
       <c r="B40" s="4"/>
       <c r="C40" s="3"/>

</xml_diff>